<commit_message>
Changes pre Convergence Study
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.6 - eq mot/Excel Files/flyball_governor/PT_flyball_governor_si.xlsx
+++ b/mbs-EP-v.1.0.6 - eq mot/Excel Files/flyball_governor/PT_flyball_governor_si.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Desktop\Thesis-Project\Multibody-System-Thesis-Software\mbs-EP-v.1.0.6 - eq mot\Excel Files\flyball_governor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFAD7A2-4C8B-45C8-A7C2-7DED637E182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D03A7A-EC67-421D-BA67-06322322AF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1980" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="256">
   <si>
     <t>Mass</t>
   </si>
@@ -1131,7 +1131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1191,7 +1191,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1879,8 +1878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,44 +1898,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="J2" s="68" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
+      <c r="J2" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="22">
+      <c r="C3" s="53"/>
+      <c r="D3" s="21">
         <v>5</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="55" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="48"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="47"/>
       <c r="P3" s="6" t="s">
         <v>152</v>
       </c>
@@ -1945,14 +1944,14 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="38">
+      <c r="C4" s="53"/>
+      <c r="D4" s="37">
         <v>1E-3</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="6" t="s">
@@ -1961,30 +1960,30 @@
       <c r="K4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="L4" s="73"/>
+      <c r="L4" s="72"/>
       <c r="M4" s="18" t="s">
         <v>123</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="O4" s="49"/>
+      <c r="O4" s="48"/>
       <c r="P4" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="Q4" s="30" t="s">
+      <c r="Q4" s="29" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="22" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>67</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -1993,30 +1992,30 @@
       <c r="K5" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="L5" s="73"/>
+      <c r="L5" s="72"/>
       <c r="M5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="49"/>
+      <c r="O5" s="48"/>
       <c r="P5" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="Q5" s="30" t="s">
+      <c r="Q5" s="29" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="22" t="s">
+      <c r="C6" s="53"/>
+      <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>76</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -2025,30 +2024,30 @@
       <c r="K6" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="73"/>
+      <c r="L6" s="72"/>
       <c r="M6" s="6" t="s">
         <v>125</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="O6" s="49"/>
+      <c r="O6" s="48"/>
       <c r="P6" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="Q6" s="30" t="s">
+      <c r="Q6" s="29" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="22">
+      <c r="C7" s="53"/>
+      <c r="D7" s="21">
         <v>-9.8066499999999994</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>102</v>
       </c>
       <c r="J7" s="6" t="s">
@@ -2057,30 +2056,30 @@
       <c r="K7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="73"/>
+      <c r="L7" s="72"/>
       <c r="M7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="49"/>
+      <c r="O7" s="48"/>
       <c r="P7" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="Q7" s="30" t="s">
+      <c r="Q7" s="29" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>82</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -2089,28 +2088,28 @@
       <c r="K8" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="L8" s="73"/>
+      <c r="L8" s="72"/>
       <c r="M8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="49"/>
+      <c r="O8" s="48"/>
       <c r="P8" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="Q8" s="30" t="s">
+      <c r="Q8" s="29" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23" t="s">
+      <c r="C9" s="53"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22" t="s">
         <v>116</v>
       </c>
       <c r="J9" s="6" t="s">
@@ -2119,18 +2118,18 @@
       <c r="K9" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="L9" s="73"/>
+      <c r="L9" s="72"/>
       <c r="M9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="49"/>
+      <c r="O9" s="48"/>
       <c r="P9" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="Q9" s="30" t="s">
+      <c r="Q9" s="29" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2141,672 +2140,662 @@
       <c r="K10" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="L10" s="73"/>
+      <c r="L10" s="72"/>
       <c r="M10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="49"/>
+      <c r="O10" s="48"/>
       <c r="P10" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="Q10" s="30" t="s">
+      <c r="Q10" s="29" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="73"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="72"/>
       <c r="M11" s="6" t="s">
         <v>127</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="O11" s="49"/>
+      <c r="O11" s="48"/>
       <c r="P11" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="Q11" s="30" t="s">
+      <c r="Q11" s="29" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="73"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="72"/>
       <c r="M12" s="6" t="s">
         <v>128</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="O12" s="49"/>
+      <c r="O12" s="48"/>
       <c r="P12" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="Q12" s="30" t="s">
+      <c r="Q12" s="29" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="6" t="s">
         <v>230</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="73"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="72"/>
       <c r="M13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="49"/>
+      <c r="O13" s="48"/>
       <c r="P13" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="Q13" s="30" t="s">
+      <c r="Q13" s="29" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="6" t="s">
-        <v>230</v>
-      </c>
+      <c r="C14" s="51"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="73"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="72"/>
       <c r="M14" s="6" t="s">
         <v>129</v>
       </c>
       <c r="N14" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="O14" s="49"/>
+      <c r="O14" s="48"/>
       <c r="P14" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="Q14" s="30" t="s">
+      <c r="Q14" s="29" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="6" t="s">
-        <v>230</v>
-      </c>
+      <c r="C15" s="51"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="J15" s="55" t="s">
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="J15" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="K15" s="56"/>
-      <c r="L15" s="73"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="72"/>
       <c r="M15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="49"/>
+      <c r="O15" s="48"/>
       <c r="P15" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="Q15" s="30" t="s">
+      <c r="Q15" s="29" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="6" t="s">
-        <v>230</v>
-      </c>
+      <c r="C16" s="51"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
       <c r="J16" s="6" t="s">
         <v>89</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="73"/>
+      <c r="L16" s="72"/>
       <c r="M16" s="6" t="s">
         <v>130</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="O16" s="49"/>
+      <c r="O16" s="48"/>
       <c r="P16" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="Q16" s="30" t="s">
+      <c r="Q16" s="29" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="6" t="s">
-        <v>230</v>
-      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
       <c r="J17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="73"/>
-      <c r="M17" s="55" t="s">
+      <c r="L17" s="72"/>
+      <c r="M17" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="N17" s="56"/>
-      <c r="O17" s="49"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="48"/>
       <c r="P17" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="Q17" s="30" t="s">
+      <c r="Q17" s="29" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="51"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="6" t="s">
         <v>230</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
       <c r="J18" s="6" t="s">
         <v>90</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="73"/>
+      <c r="L18" s="72"/>
       <c r="M18" s="18" t="s">
         <v>151</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="O18" s="49"/>
+      <c r="O18" s="48"/>
       <c r="P18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="Q18" s="30" t="s">
+      <c r="Q18" s="29" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="51"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="6"/>
       <c r="E19" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
       <c r="J19" s="6" t="s">
         <v>91</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="73"/>
+      <c r="L19" s="72"/>
       <c r="M19" s="19" t="s">
         <v>143</v>
       </c>
       <c r="N19" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="O19" s="49"/>
+      <c r="O19" s="48"/>
       <c r="P19" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="Q19" s="30" t="s">
+      <c r="Q19" s="29" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="20" t="s">
-        <v>230</v>
-      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
       <c r="J20" s="6" t="s">
         <v>97</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="L20" s="73"/>
+      <c r="L20" s="72"/>
       <c r="M20" s="19" t="s">
         <v>144</v>
       </c>
       <c r="N20" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="49"/>
+      <c r="O20" s="48"/>
       <c r="P20" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="Q20" s="30" t="s">
+      <c r="Q20" s="29" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="51" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="21"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
       <c r="J21" s="6" t="s">
         <v>92</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="L21" s="73"/>
+      <c r="L21" s="72"/>
       <c r="M21" s="19" t="s">
         <v>145</v>
       </c>
       <c r="N21" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="O21" s="49"/>
+      <c r="O21" s="48"/>
       <c r="P21" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="Q21" s="30" t="s">
+      <c r="Q21" s="29" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C22" s="59"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="6">
         <v>5</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="F22" s="67" t="s">
+      <c r="F22" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="G22" s="67"/>
-      <c r="H22" s="37"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="36"/>
       <c r="J22" s="6" t="s">
         <v>103</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="L22" s="74"/>
+      <c r="L22" s="73"/>
       <c r="M22" s="19" t="s">
         <v>146</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="O22" s="49"/>
+      <c r="O22" s="48"/>
       <c r="P22" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="Q22" s="30" t="s">
+      <c r="Q22" s="29" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="60"/>
-      <c r="C23" s="61"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="37"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="49"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="36"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="48"/>
       <c r="P23" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="Q23" s="30" t="s">
+      <c r="Q23" s="29" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="37"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="49"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="36"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="48"/>
       <c r="P24" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="Q24" s="30" t="s">
+      <c r="Q24" s="29" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="37"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="49"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="36"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="48"/>
       <c r="P25" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="Q25" s="30" t="s">
+      <c r="Q25" s="29" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="60"/>
-      <c r="C26" s="61"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="37"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="49"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="36"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="48"/>
       <c r="P26" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="Q26" s="30" t="s">
+      <c r="Q26" s="29" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="37"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="49"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="36"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="48"/>
       <c r="P27" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="Q27" s="30" t="s">
+      <c r="Q27" s="29" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="37"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="49"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="36"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="48"/>
       <c r="P28" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="Q28" s="30" t="s">
+      <c r="Q28" s="29" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="62"/>
-      <c r="C29" s="63"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="62"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="37"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="49"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="36"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="48"/>
       <c r="P29" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="Q29" s="30" t="s">
+      <c r="Q29" s="29" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="42"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="49"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="48"/>
       <c r="P30" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="Q30" s="30" t="s">
+      <c r="Q30" s="29" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="42"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="49"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="48"/>
       <c r="P31" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="Q31" s="30" t="s">
+      <c r="Q31" s="29" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="42"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="49"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="48"/>
       <c r="P32" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="Q32" s="30" t="s">
+      <c r="Q32" s="29" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="42"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="49"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="48"/>
       <c r="P33" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="Q33" s="30" t="s">
+      <c r="Q33" s="29" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="42"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="49"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="48"/>
       <c r="P34" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="Q34" s="30" t="s">
+      <c r="Q34" s="29" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="42"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="49"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="48"/>
       <c r="P35" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="Q35" s="30" t="s">
+      <c r="Q35" s="29" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="42"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="49"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="48"/>
       <c r="P36" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="Q36" s="30" t="s">
+      <c r="Q36" s="29" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="42"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="44"/>
-      <c r="O37" s="49"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="48"/>
       <c r="P37" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="Q37" s="30" t="s">
+      <c r="Q37" s="29" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="45"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="49"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="48"/>
       <c r="P38" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="Q38" s="30" t="s">
+      <c r="Q38" s="29" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2814,7 +2803,7 @@
       <c r="P39" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="Q39" s="30" t="s">
+      <c r="Q39" s="29" t="s">
         <v>224</v>
       </c>
     </row>
@@ -2861,7 +2850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -2882,118 +2871,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="52" t="s">
+      <c r="A1" s="56"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52" t="s">
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52" t="s">
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52" t="s">
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="52"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="52" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52" t="s">
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52" t="s">
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="67" t="s">
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="52" t="s">
+      <c r="S2" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52" t="s">
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="50" t="s">
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="52" t="s">
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52" t="s">
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52" t="s">
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -3047,8 +3036,8 @@
       <c r="Q3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="67"/>
-      <c r="S3" s="76"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="75"/>
       <c r="T3" s="6" t="s">
         <v>58</v>
       </c>
@@ -6695,16 +6684,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
@@ -6729,11 +6718,11 @@
       <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6789,19 +6778,19 @@
       <c r="X4" s="5"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
@@ -6826,16 +6815,16 @@
       <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="83" t="s">
+      <c r="F6" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="84"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="83" t="s">
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="85"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="84"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -6871,22 +6860,22 @@
       <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
@@ -6911,21 +6900,21 @@
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="79" t="s">
+      <c r="F9" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="77" t="s">
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77" t="s">
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76" t="s">
         <v>240</v>
       </c>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -6978,19 +6967,19 @@
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
@@ -7015,16 +7004,16 @@
       <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="77" t="s">
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
@@ -7091,7 +7080,7 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <v>0.05</v>
       </c>
       <c r="G15" s="1">
@@ -7100,7 +7089,7 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="31">
         <v>0.05</v>
       </c>
       <c r="J15" s="7">
@@ -7126,7 +7115,7 @@
       <c r="E16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="32">
         <v>-0.05</v>
       </c>
       <c r="G16" s="1">
@@ -7135,7 +7124,7 @@
       <c r="H16" s="1">
         <v>0</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="31">
         <v>-0.05</v>
       </c>
       <c r="J16" s="7">
@@ -7166,19 +7155,19 @@
       <c r="X17" s="5"/>
     </row>
     <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="77"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
@@ -7203,16 +7192,16 @@
       <c r="E19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="79" t="s">
+      <c r="F19" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="77" t="s">
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
     </row>
     <row r="20" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -7248,19 +7237,19 @@
       <c r="X21" s="5"/>
     </row>
     <row r="22" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="77"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
@@ -7285,16 +7274,16 @@
       <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="79" t="s">
+      <c r="F23" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="77" t="s">
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
+      <c r="J23" s="76"/>
+      <c r="K23" s="76"/>
     </row>
     <row r="24" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
@@ -7333,22 +7322,22 @@
     </row>
     <row r="25" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:24" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="78"/>
-      <c r="L26" s="78"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="78"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
     </row>
     <row r="27" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -7366,44 +7355,44 @@
       <c r="E27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="79" t="s">
+      <c r="F27" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="77" t="s">
+      <c r="G27" s="78"/>
+      <c r="H27" s="78"/>
+      <c r="I27" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77" t="s">
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76" t="s">
         <v>118</v>
       </c>
-      <c r="M27" s="77"/>
-      <c r="N27" s="77"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="76"/>
     </row>
     <row r="28" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:24" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="78"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="78"/>
-      <c r="P30" s="78"/>
-      <c r="Q30" s="78"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
     </row>
     <row r="31" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -7421,26 +7410,26 @@
       <c r="E31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="83" t="s">
+      <c r="F31" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="84"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="83" t="s">
+      <c r="G31" s="83"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="J31" s="84"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="77" t="s">
+      <c r="J31" s="83"/>
+      <c r="K31" s="84"/>
+      <c r="L31" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="M31" s="77"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77" t="s">
+      <c r="M31" s="76"/>
+      <c r="N31" s="76"/>
+      <c r="O31" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="77"/>
+      <c r="P31" s="76"/>
+      <c r="Q31" s="76"/>
     </row>
     <row r="32" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F32" s="9"/>
@@ -7464,14 +7453,14 @@
       <c r="R33"/>
     </row>
     <row r="34" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
@@ -7545,12 +7534,12 @@
       <c r="X37" s="5"/>
     </row>
     <row r="38" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="78" t="s">
+      <c r="A38" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="78"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
       <c r="U38" s="5"/>
@@ -7604,15 +7593,15 @@
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="80" t="s">
+      <c r="A42" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="82"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="81"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
@@ -7627,11 +7616,11 @@
       <c r="D43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="77" t="s">
+      <c r="E43" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="77"/>
-      <c r="G43" s="77"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
     </row>
     <row r="44" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -7870,21 +7859,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86" t="s">
         <v>248</v>
       </c>
-      <c r="K1" s="87"/>
+      <c r="K1" s="86"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -7902,11 +7891,11 @@
       <c r="E2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
       <c r="I2" s="4" t="s">
         <v>245</v>
       </c>
@@ -7979,58 +7968,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
     </row>
     <row r="2" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="88" t="s">
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="87" t="s">
         <v>238</v>
       </c>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="90"/>
-      <c r="AB2" s="102" t="s">
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="89"/>
+      <c r="AB2" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="AC2" s="103"/>
-      <c r="AD2" s="103"/>
-      <c r="AE2" s="103"/>
-      <c r="AF2" s="103"/>
-      <c r="AG2" s="104"/>
+      <c r="AC2" s="102"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AF2" s="102"/>
+      <c r="AG2" s="103"/>
     </row>
     <row r="3" spans="1:33" s="12" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -8048,17 +8037,17 @@
       <c r="E3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="91" t="s">
+      <c r="G3" s="97"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="31" t="s">
+      <c r="J3" s="91"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="30" t="s">
         <v>233</v>
       </c>
       <c r="M3" s="14" t="s">
@@ -8076,16 +8065,16 @@
       <c r="Q3" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="R3" s="100" t="s">
+      <c r="R3" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="S3" s="100"/>
-      <c r="AB3" s="105"/>
-      <c r="AC3" s="106"/>
-      <c r="AD3" s="106"/>
-      <c r="AE3" s="106"/>
-      <c r="AF3" s="106"/>
-      <c r="AG3" s="107"/>
+      <c r="S3" s="99"/>
+      <c r="AB3" s="104"/>
+      <c r="AC3" s="105"/>
+      <c r="AD3" s="105"/>
+      <c r="AE3" s="105"/>
+      <c r="AF3" s="105"/>
+      <c r="AG3" s="106"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -8098,7 +8087,7 @@
       <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>0.05</v>
       </c>
       <c r="G4" s="1">
@@ -8107,7 +8096,7 @@
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="32">
         <v>0.48303000000000001</v>
       </c>
       <c r="J4" s="1">
@@ -8119,7 +8108,7 @@
       <c r="L4" s="1">
         <v>0.5</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="31">
         <v>800000</v>
       </c>
       <c r="N4" s="15"/>
@@ -8127,12 +8116,12 @@
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
-      <c r="AB4" s="105"/>
-      <c r="AC4" s="106"/>
-      <c r="AD4" s="106"/>
-      <c r="AE4" s="106"/>
-      <c r="AF4" s="106"/>
-      <c r="AG4" s="107"/>
+      <c r="AB4" s="104"/>
+      <c r="AC4" s="105"/>
+      <c r="AD4" s="105"/>
+      <c r="AE4" s="105"/>
+      <c r="AF4" s="105"/>
+      <c r="AG4" s="106"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -8146,7 +8135,7 @@
       <c r="E5" s="1">
         <v>4</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>-0.05</v>
       </c>
       <c r="G5" s="1">
@@ -8155,7 +8144,7 @@
       <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="32">
         <v>-0.48303000000000001</v>
       </c>
       <c r="J5" s="1">
@@ -8167,7 +8156,7 @@
       <c r="L5" s="1">
         <v>0.5</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="31">
         <v>800000</v>
       </c>
       <c r="N5" s="1"/>
@@ -8176,76 +8165,76 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="AB5" s="105"/>
-      <c r="AC5" s="106"/>
-      <c r="AD5" s="106"/>
-      <c r="AE5" s="106"/>
-      <c r="AF5" s="106"/>
-      <c r="AG5" s="107"/>
+      <c r="AB5" s="104"/>
+      <c r="AC5" s="105"/>
+      <c r="AD5" s="105"/>
+      <c r="AE5" s="105"/>
+      <c r="AF5" s="105"/>
+      <c r="AG5" s="106"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AB6" s="105"/>
-      <c r="AC6" s="106"/>
-      <c r="AD6" s="106"/>
-      <c r="AE6" s="106"/>
-      <c r="AF6" s="106"/>
-      <c r="AG6" s="107"/>
+      <c r="AB6" s="104"/>
+      <c r="AC6" s="105"/>
+      <c r="AD6" s="105"/>
+      <c r="AE6" s="105"/>
+      <c r="AF6" s="105"/>
+      <c r="AG6" s="106"/>
     </row>
     <row r="7" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="87"/>
-      <c r="R7" s="87"/>
-      <c r="AB7" s="105"/>
-      <c r="AC7" s="106"/>
-      <c r="AD7" s="106"/>
-      <c r="AE7" s="106"/>
-      <c r="AF7" s="106"/>
-      <c r="AG7" s="107"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="86"/>
+      <c r="O7" s="86"/>
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="AB7" s="104"/>
+      <c r="AC7" s="105"/>
+      <c r="AD7" s="105"/>
+      <c r="AE7" s="105"/>
+      <c r="AF7" s="105"/>
+      <c r="AG7" s="106"/>
     </row>
     <row r="8" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="78"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="101" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="O8" s="101"/>
-      <c r="P8" s="101"/>
-      <c r="Q8" s="101"/>
-      <c r="R8" s="101"/>
-      <c r="AB8" s="105"/>
-      <c r="AC8" s="106"/>
-      <c r="AD8" s="106"/>
-      <c r="AE8" s="106"/>
-      <c r="AF8" s="106"/>
-      <c r="AG8" s="107"/>
+      <c r="O8" s="100"/>
+      <c r="P8" s="100"/>
+      <c r="Q8" s="100"/>
+      <c r="R8" s="100"/>
+      <c r="AB8" s="104"/>
+      <c r="AC8" s="105"/>
+      <c r="AD8" s="105"/>
+      <c r="AE8" s="105"/>
+      <c r="AF8" s="105"/>
+      <c r="AG8" s="106"/>
     </row>
     <row r="9" spans="1:33" s="12" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -8263,16 +8252,16 @@
       <c r="E9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="91" t="s">
+      <c r="G9" s="97"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="92"/>
-      <c r="K9" s="93"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="92"/>
       <c r="L9" s="14" t="s">
         <v>107</v>
       </c>
@@ -8288,16 +8277,16 @@
       <c r="P9" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="Q9" s="97" t="s">
+      <c r="Q9" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="R9" s="99"/>
-      <c r="AB9" s="105"/>
-      <c r="AC9" s="106"/>
-      <c r="AD9" s="106"/>
-      <c r="AE9" s="106"/>
-      <c r="AF9" s="106"/>
-      <c r="AG9" s="107"/>
+      <c r="R9" s="98"/>
+      <c r="AB9" s="104"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="106"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -8311,7 +8300,7 @@
       <c r="E10" s="1">
         <v>3</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <v>0.05</v>
       </c>
       <c r="G10" s="1">
@@ -8320,7 +8309,7 @@
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="32">
         <v>0.48303000000000001</v>
       </c>
       <c r="J10" s="1">
@@ -8329,16 +8318,16 @@
       <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="32">
         <v>40000</v>
       </c>
       <c r="M10" s="10"/>
-      <c r="AB10" s="105"/>
-      <c r="AC10" s="106"/>
-      <c r="AD10" s="106"/>
-      <c r="AE10" s="106"/>
-      <c r="AF10" s="106"/>
-      <c r="AG10" s="107"/>
+      <c r="AB10" s="104"/>
+      <c r="AC10" s="105"/>
+      <c r="AD10" s="105"/>
+      <c r="AE10" s="105"/>
+      <c r="AF10" s="105"/>
+      <c r="AG10" s="106"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -8352,7 +8341,7 @@
       <c r="E11" s="1">
         <v>4</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="32">
         <v>-0.05</v>
       </c>
       <c r="G11" s="1">
@@ -8361,7 +8350,7 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="32">
         <v>-0.48303000000000001</v>
       </c>
       <c r="J11" s="1">
@@ -8370,90 +8359,90 @@
       <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="32">
         <v>40000</v>
       </c>
-      <c r="AB11" s="105"/>
-      <c r="AC11" s="106"/>
-      <c r="AD11" s="106"/>
-      <c r="AE11" s="106"/>
-      <c r="AF11" s="106"/>
-      <c r="AG11" s="107"/>
+      <c r="AB11" s="104"/>
+      <c r="AC11" s="105"/>
+      <c r="AD11" s="105"/>
+      <c r="AE11" s="105"/>
+      <c r="AF11" s="105"/>
+      <c r="AG11" s="106"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Q12" s="1"/>
-      <c r="AB12" s="105"/>
-      <c r="AC12" s="106"/>
-      <c r="AD12" s="106"/>
-      <c r="AE12" s="106"/>
-      <c r="AF12" s="106"/>
-      <c r="AG12" s="107"/>
+      <c r="AB12" s="104"/>
+      <c r="AC12" s="105"/>
+      <c r="AD12" s="105"/>
+      <c r="AE12" s="105"/>
+      <c r="AF12" s="105"/>
+      <c r="AG12" s="106"/>
     </row>
     <row r="13" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="87"/>
-      <c r="T13" s="87"/>
-      <c r="U13" s="87"/>
-      <c r="V13" s="87"/>
-      <c r="W13" s="87"/>
-      <c r="X13" s="87"/>
-      <c r="Y13" s="87"/>
-      <c r="AB13" s="108"/>
-      <c r="AC13" s="109"/>
-      <c r="AD13" s="109"/>
-      <c r="AE13" s="109"/>
-      <c r="AF13" s="109"/>
-      <c r="AG13" s="110"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
+      <c r="V13" s="86"/>
+      <c r="W13" s="86"/>
+      <c r="X13" s="86"/>
+      <c r="Y13" s="86"/>
+      <c r="AB13" s="107"/>
+      <c r="AC13" s="108"/>
+      <c r="AD13" s="108"/>
+      <c r="AE13" s="108"/>
+      <c r="AF13" s="108"/>
+      <c r="AG13" s="109"/>
     </row>
     <row r="14" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="80"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="81"/>
-      <c r="S14" s="82"/>
-      <c r="T14" s="88" t="s">
+      <c r="A14" s="79"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="80"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="U14" s="89"/>
-      <c r="V14" s="89"/>
-      <c r="W14" s="89"/>
-      <c r="X14" s="89"/>
-      <c r="Y14" s="90"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="34"/>
+      <c r="U14" s="88"/>
+      <c r="V14" s="88"/>
+      <c r="W14" s="88"/>
+      <c r="X14" s="88"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="33"/>
     </row>
     <row r="15" spans="1:33" s="12" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -8471,26 +8460,26 @@
       <c r="E15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="75" t="s">
         <v>241</v>
       </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="91" t="s">
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="90" t="s">
         <v>242</v>
       </c>
-      <c r="J15" s="92"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="94" t="s">
+      <c r="J15" s="91"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="93" t="s">
         <v>243</v>
       </c>
-      <c r="M15" s="95"/>
-      <c r="N15" s="96"/>
-      <c r="O15" s="94" t="s">
+      <c r="M15" s="94"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="93" t="s">
         <v>244</v>
       </c>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="96"/>
+      <c r="P15" s="94"/>
+      <c r="Q15" s="95"/>
       <c r="R15" s="14" t="s">
         <v>70</v>
       </c>
@@ -8509,10 +8498,10 @@
       <c r="W15" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="X15" s="97" t="s">
+      <c r="X15" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="Y15" s="99"/>
+      <c r="Y15" s="98"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -8559,46 +8548,46 @@
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
-      <c r="Q18" s="87"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="86"/>
     </row>
     <row r="19" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="88" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="87" t="s">
         <v>238</v>
       </c>
-      <c r="M19" s="89"/>
-      <c r="N19" s="89"/>
-      <c r="O19" s="89"/>
-      <c r="P19" s="89"/>
-      <c r="Q19" s="90"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
+      <c r="O19" s="88"/>
+      <c r="P19" s="88"/>
+      <c r="Q19" s="89"/>
     </row>
     <row r="20" spans="1:20" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
@@ -8616,16 +8605,16 @@
       <c r="E20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="76" t="s">
+      <c r="F20" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="94" t="s">
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="93" t="s">
         <v>150</v>
       </c>
-      <c r="J20" s="95"/>
-      <c r="K20" s="96"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="95"/>
       <c r="L20" s="11" t="s">
         <v>108</v>
       </c>
@@ -8638,10 +8627,10 @@
       <c r="O20" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="P20" s="97" t="s">
+      <c r="P20" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="Q20" s="99"/>
+      <c r="Q20" s="98"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -8735,21 +8724,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="F1" s="69" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="F1" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="71"/>
-      <c r="I1" s="69" t="s">
+      <c r="G1" s="70"/>
+      <c r="I1" s="68" t="s">
         <v>229</v>
       </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="71"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="70"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -8767,12 +8756,12 @@
       <c r="G2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="111" t="s">
+      <c r="I2" s="110" t="s">
         <v>228</v>
       </c>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -8781,13 +8770,13 @@
       <c r="F3" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -8796,13 +8785,13 @@
       <c r="F4" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="110"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -8811,13 +8800,13 @@
       <c r="F5" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="110"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -8826,13 +8815,13 @@
       <c r="F6" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
@@ -8842,7 +8831,7 @@
       <c r="F7" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>165</v>
       </c>
       <c r="H7" s="7"/>
@@ -8854,7 +8843,7 @@
       <c r="F8" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>166</v>
       </c>
     </row>
@@ -8866,7 +8855,7 @@
       <c r="F9" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>167</v>
       </c>
       <c r="H9" s="1"/>
@@ -8878,7 +8867,7 @@
       <c r="F10" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>168</v>
       </c>
     </row>
@@ -8889,7 +8878,7 @@
       <c r="F11" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="29" t="s">
         <v>173</v>
       </c>
     </row>
@@ -8900,7 +8889,7 @@
       <c r="F12" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="29" t="s">
         <v>174</v>
       </c>
     </row>
@@ -8911,7 +8900,7 @@
       <c r="F13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="29" t="s">
         <v>175</v>
       </c>
     </row>
@@ -8922,7 +8911,7 @@
       <c r="F14" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="29" t="s">
         <v>176</v>
       </c>
     </row>
@@ -8933,7 +8922,7 @@
       <c r="F15" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="29" t="s">
         <v>181</v>
       </c>
     </row>
@@ -8944,7 +8933,7 @@
       <c r="F16" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="29" t="s">
         <v>182</v>
       </c>
     </row>
@@ -8955,7 +8944,7 @@
       <c r="F17" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="29" t="s">
         <v>183</v>
       </c>
     </row>
@@ -8966,7 +8955,7 @@
       <c r="F18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="29" t="s">
         <v>184</v>
       </c>
     </row>
@@ -8977,7 +8966,7 @@
       <c r="F19" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="29" t="s">
         <v>189</v>
       </c>
     </row>
@@ -8988,7 +8977,7 @@
       <c r="F20" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="29" t="s">
         <v>190</v>
       </c>
     </row>
@@ -8999,7 +8988,7 @@
       <c r="F21" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="29" t="s">
         <v>191</v>
       </c>
     </row>
@@ -9010,7 +8999,7 @@
       <c r="F22" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="29" t="s">
         <v>192</v>
       </c>
     </row>
@@ -9021,7 +9010,7 @@
       <c r="F23" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="29" t="s">
         <v>193</v>
       </c>
     </row>
@@ -9032,7 +9021,7 @@
       <c r="F24" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="29" t="s">
         <v>195</v>
       </c>
     </row>
@@ -9043,7 +9032,7 @@
       <c r="F25" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="29" t="s">
         <v>196</v>
       </c>
     </row>
@@ -9054,7 +9043,7 @@
       <c r="F26" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G26" s="29" t="s">
         <v>197</v>
       </c>
     </row>
@@ -9065,7 +9054,7 @@
       <c r="F27" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="29" t="s">
         <v>209</v>
       </c>
     </row>
@@ -9076,7 +9065,7 @@
       <c r="F28" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="29" t="s">
         <v>210</v>
       </c>
     </row>
@@ -9087,7 +9076,7 @@
       <c r="F29" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="29" t="s">
         <v>211</v>
       </c>
     </row>
@@ -9098,7 +9087,7 @@
       <c r="F30" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="29" t="s">
         <v>212</v>
       </c>
     </row>
@@ -9109,7 +9098,7 @@
       <c r="F31" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="29" t="s">
         <v>213</v>
       </c>
     </row>
@@ -9120,7 +9109,7 @@
       <c r="F32" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="G32" s="30" t="s">
+      <c r="G32" s="29" t="s">
         <v>214</v>
       </c>
     </row>
@@ -9131,7 +9120,7 @@
       <c r="F33" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="G33" s="30" t="s">
+      <c r="G33" s="29" t="s">
         <v>215</v>
       </c>
     </row>
@@ -9142,7 +9131,7 @@
       <c r="F34" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="29" t="s">
         <v>216</v>
       </c>
     </row>
@@ -9153,7 +9142,7 @@
       <c r="F35" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="29" t="s">
         <v>221</v>
       </c>
     </row>
@@ -9164,7 +9153,7 @@
       <c r="F36" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G36" s="29" t="s">
         <v>222</v>
       </c>
     </row>
@@ -9175,7 +9164,7 @@
       <c r="F37" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="29" t="s">
         <v>223</v>
       </c>
     </row>
@@ -9186,7 +9175,7 @@
       <c r="F38" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="G38" s="30" t="s">
+      <c r="G38" s="29" t="s">
         <v>224</v>
       </c>
     </row>

</xml_diff>